<commit_message>
Adding support for Row.getFirstCellNum() (#49)
</commit_message>
<xml_diff>
--- a/src/test/resources/gaps.xlsx
+++ b/src/test/resources/gaps.xlsx
@@ -11,11 +11,16 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Dat</t>
   </si>
@@ -27,6 +32,9 @@
   </si>
   <si>
     <t>!</t>
+  </si>
+  <si>
+    <t>WUT</t>
   </si>
 </sst>
 </file>
@@ -41,6 +49,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -122,16 +131,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:G7"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -149,6 +155,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D10" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>